<commit_message>
fixed NoneType object recipe;
</commit_message>
<xml_diff>
--- a/static/Results.xlsx
+++ b/static/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -25,10 +25,19 @@
     <t>Cost</t>
   </si>
   <si>
+    <t>Лук 100г</t>
+  </si>
+  <si>
+    <t>Перец молотый 10г</t>
+  </si>
+  <si>
+    <t>Соль</t>
+  </si>
+  <si>
     <t>Total:</t>
   </si>
   <si>
-    <t>0 Rubles</t>
+    <t>155 Rubles</t>
   </si>
 </sst>
 </file>
@@ -386,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,10 +420,52 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>